<commit_message>
Add Header in export display
</commit_message>
<xml_diff>
--- a/application/controllers/Items.xlsx
+++ b/application/controllers/Items.xlsx
@@ -60,6 +60,41 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="714375" cy="714375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,7 +394,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1"/>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -372,5 +411,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>